<commit_message>
Figure 2 data pos and neg
</commit_message>
<xml_diff>
--- a/rawdata/supplementary_material_V2.xlsx
+++ b/rawdata/supplementary_material_V2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20372"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DECD5CD0-2EFF-4947-A5A7-01CF9206DEDE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59CA92B-E477-47EF-A9E5-77C0DB502C57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="765" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="765" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scoring system" sheetId="1" r:id="rId1"/>
@@ -5648,12 +5648,6 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5663,11 +5657,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5675,10 +5669,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5688,12 +5694,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6146,10 +6146,10 @@
       <c r="D3" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="107" t="s">
+      <c r="E3" s="109" t="s">
         <v>631</v>
       </c>
-      <c r="F3" s="107" t="s">
+      <c r="F3" s="109" t="s">
         <v>632</v>
       </c>
     </row>
@@ -6166,8 +6166,8 @@
       <c r="D4" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="107"/>
-      <c r="F4" s="107"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="109"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
@@ -6292,10 +6292,10 @@
       <c r="D11" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="107" t="s">
+      <c r="E11" s="109" t="s">
         <v>641</v>
       </c>
-      <c r="F11" s="107" t="s">
+      <c r="F11" s="109" t="s">
         <v>642</v>
       </c>
     </row>
@@ -6312,8 +6312,8 @@
       <c r="D12" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="107"/>
-      <c r="F12" s="107"/>
+      <c r="E12" s="109"/>
+      <c r="F12" s="109"/>
     </row>
     <row r="13" spans="1:6" ht="211.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -6328,8 +6328,8 @@
       <c r="D13" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="107"/>
-      <c r="F13" s="107"/>
+      <c r="E13" s="109"/>
+      <c r="F13" s="109"/>
     </row>
     <row r="14" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
@@ -6454,10 +6454,10 @@
       <c r="D20" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="107" t="s">
+      <c r="E20" s="109" t="s">
         <v>645</v>
       </c>
-      <c r="F20" s="107" t="s">
+      <c r="F20" s="109" t="s">
         <v>646</v>
       </c>
     </row>
@@ -6474,8 +6474,8 @@
       <c r="D21" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="107"/>
-      <c r="F21" s="107"/>
+      <c r="E21" s="109"/>
+      <c r="F21" s="109"/>
     </row>
     <row r="22" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
@@ -7400,10 +7400,10 @@
       <c r="D70" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E70" s="107" t="s">
+      <c r="E70" s="109" t="s">
         <v>652</v>
       </c>
-      <c r="F70" s="107" t="s">
+      <c r="F70" s="109" t="s">
         <v>653</v>
       </c>
     </row>
@@ -7420,8 +7420,8 @@
       <c r="D71" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E71" s="107"/>
-      <c r="F71" s="107"/>
+      <c r="E71" s="109"/>
+      <c r="F71" s="109"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
@@ -7706,10 +7706,10 @@
       <c r="D86" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E86" s="104" t="s">
+      <c r="E86" s="102" t="s">
         <v>659</v>
       </c>
-      <c r="F86" s="104" t="s">
+      <c r="F86" s="102" t="s">
         <v>660</v>
       </c>
     </row>
@@ -7726,8 +7726,8 @@
       <c r="D87" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E87" s="104"/>
-      <c r="F87" s="104"/>
+      <c r="E87" s="102"/>
+      <c r="F87" s="102"/>
     </row>
     <row r="88" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A88" s="24" t="s">
@@ -7742,8 +7742,8 @@
       <c r="D88" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E88" s="104"/>
-      <c r="F88" s="104"/>
+      <c r="E88" s="102"/>
+      <c r="F88" s="102"/>
     </row>
     <row r="89" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A89" s="24" t="s">
@@ -8228,10 +8228,10 @@
       <c r="D114" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="107" t="s">
+      <c r="E114" s="109" t="s">
         <v>663</v>
       </c>
-      <c r="F114" s="107" t="s">
+      <c r="F114" s="109" t="s">
         <v>308</v>
       </c>
     </row>
@@ -8248,8 +8248,8 @@
       <c r="D115" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="107"/>
-      <c r="F115" s="107"/>
+      <c r="E115" s="109"/>
+      <c r="F115" s="109"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="24" t="s">
@@ -9012,10 +9012,10 @@
       <c r="D156" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E156" s="107" t="s">
+      <c r="E156" s="109" t="s">
         <v>682</v>
       </c>
-      <c r="F156" s="107" t="s">
+      <c r="F156" s="109" t="s">
         <v>658</v>
       </c>
     </row>
@@ -9032,8 +9032,8 @@
       <c r="D157" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E157" s="107"/>
-      <c r="F157" s="107"/>
+      <c r="E157" s="109"/>
+      <c r="F157" s="109"/>
     </row>
     <row r="158" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A158" s="24" t="s">
@@ -9237,12 +9237,19 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="E156:E157"/>
+    <mergeCell ref="F156:F157"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="E114:E115"/>
+    <mergeCell ref="F114:F115"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A155:F155"/>
     <mergeCell ref="E86:E88"/>
     <mergeCell ref="F86:F88"/>
     <mergeCell ref="A19:F19"/>
@@ -9256,19 +9263,12 @@
     <mergeCell ref="E70:E71"/>
     <mergeCell ref="F70:F71"/>
     <mergeCell ref="A82:F82"/>
-    <mergeCell ref="E156:E157"/>
-    <mergeCell ref="F156:F157"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="E114:E115"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9481,10 +9481,10 @@
       <c r="D11" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="104" t="s">
+      <c r="E11" s="102" t="s">
         <v>730</v>
       </c>
-      <c r="F11" s="105" t="s">
+      <c r="F11" s="103" t="s">
         <v>731</v>
       </c>
     </row>
@@ -9501,8 +9501,8 @@
       <c r="D12" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="104"/>
-      <c r="F12" s="106"/>
+      <c r="E12" s="102"/>
+      <c r="F12" s="104"/>
     </row>
     <row r="13" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -12454,6 +12454,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
     <mergeCell ref="A91:F91"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A10:F10"/>
@@ -12466,14 +12474,6 @@
     <mergeCell ref="A63:F63"/>
     <mergeCell ref="A69:F69"/>
     <mergeCell ref="A82:F82"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -12686,10 +12686,10 @@
       <c r="D11" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="109" t="s">
+      <c r="E11" s="107" t="s">
         <v>736</v>
       </c>
-      <c r="F11" s="109" t="s">
+      <c r="F11" s="107" t="s">
         <v>737</v>
       </c>
     </row>
@@ -12706,8 +12706,8 @@
       <c r="D12" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="110"/>
-      <c r="F12" s="110"/>
+      <c r="E12" s="108"/>
+      <c r="F12" s="108"/>
     </row>
     <row r="13" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -12850,10 +12850,10 @@
       <c r="D20" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="109" t="s">
+      <c r="E20" s="107" t="s">
         <v>738</v>
       </c>
-      <c r="F20" s="109" t="s">
+      <c r="F20" s="107" t="s">
         <v>739</v>
       </c>
     </row>
@@ -12870,8 +12870,8 @@
       <c r="D21" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="110"/>
-      <c r="F21" s="110"/>
+      <c r="E21" s="108"/>
+      <c r="F21" s="108"/>
     </row>
     <row r="22" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
@@ -13796,10 +13796,10 @@
       <c r="D70" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="109" t="s">
+      <c r="E70" s="107" t="s">
         <v>746</v>
       </c>
-      <c r="F70" s="109" t="s">
+      <c r="F70" s="107" t="s">
         <v>747</v>
       </c>
     </row>
@@ -13816,8 +13816,8 @@
       <c r="D71" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E71" s="110"/>
-      <c r="F71" s="110"/>
+      <c r="E71" s="108"/>
+      <c r="F71" s="108"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
@@ -15022,10 +15022,10 @@
       <c r="D135" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E135" s="109" t="s">
+      <c r="E135" s="107" t="s">
         <v>759</v>
       </c>
-      <c r="F135" s="109" t="s">
+      <c r="F135" s="107" t="s">
         <v>749</v>
       </c>
     </row>
@@ -15042,8 +15042,8 @@
       <c r="D136" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E136" s="110"/>
-      <c r="F136" s="110"/>
+      <c r="E136" s="108"/>
+      <c r="F136" s="108"/>
     </row>
     <row r="137" spans="1:6" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A137" s="24" t="s">
@@ -15647,11 +15647,13 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="E135:E136"/>
-    <mergeCell ref="F135:F136"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A19:F19"/>
     <mergeCell ref="E126:E127"/>
     <mergeCell ref="F126:F127"/>
     <mergeCell ref="A33:F33"/>
@@ -15666,13 +15668,11 @@
     <mergeCell ref="A102:F102"/>
     <mergeCell ref="A113:F113"/>
     <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="E135:E136"/>
+    <mergeCell ref="F135:F136"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A155:F155"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15714,14 +15714,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="105" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
+      <c r="B2" s="106"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
     </row>
     <row r="3" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
@@ -18074,10 +18074,10 @@
       <c r="D126" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E126" s="104" t="s">
+      <c r="E126" s="102" t="s">
         <v>470</v>
       </c>
-      <c r="F126" s="105" t="s">
+      <c r="F126" s="103" t="s">
         <v>471</v>
       </c>
     </row>
@@ -18094,8 +18094,8 @@
       <c r="D127" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E127" s="104"/>
-      <c r="F127" s="106"/>
+      <c r="E127" s="102"/>
+      <c r="F127" s="104"/>
     </row>
     <row r="128" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A128" s="24" t="s">
@@ -18869,6 +18869,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
     <mergeCell ref="A155:F155"/>
     <mergeCell ref="A63:F63"/>
     <mergeCell ref="A69:F69"/>
@@ -18881,12 +18887,6 @@
     <mergeCell ref="F126:F127"/>
     <mergeCell ref="A131:F131"/>
     <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18896,7 +18896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6535A64-0113-4925-BB3F-009252BF36D5}">
   <dimension ref="A1:F167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A161" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E175" sqref="E175"/>
     </sheetView>
   </sheetViews>
@@ -18950,10 +18950,10 @@
       <c r="D3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="104" t="s">
+      <c r="E3" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="104" t="s">
+      <c r="F3" s="102" t="s">
         <v>28</v>
       </c>
     </row>
@@ -18970,8 +18970,8 @@
       <c r="D4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="104"/>
-      <c r="F4" s="104"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
     </row>
     <row r="5" spans="1:6" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
@@ -19096,10 +19096,10 @@
       <c r="D11" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="107" t="s">
+      <c r="E11" s="109" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="107" t="s">
+      <c r="F11" s="109" t="s">
         <v>53</v>
       </c>
     </row>
@@ -19116,8 +19116,8 @@
       <c r="D12" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="107"/>
-      <c r="F12" s="107"/>
+      <c r="E12" s="109"/>
+      <c r="F12" s="109"/>
     </row>
     <row r="13" spans="1:6" ht="15.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -19132,8 +19132,8 @@
       <c r="D13" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="107"/>
-      <c r="F13" s="107"/>
+      <c r="E13" s="109"/>
+      <c r="F13" s="109"/>
     </row>
     <row r="14" spans="1:6" ht="228.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
@@ -20200,10 +20200,10 @@
       <c r="D70" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="104" t="s">
+      <c r="E70" s="102" t="s">
         <v>201</v>
       </c>
-      <c r="F70" s="104" t="s">
+      <c r="F70" s="102" t="s">
         <v>202</v>
       </c>
     </row>
@@ -20220,8 +20220,8 @@
       <c r="D71" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E71" s="104"/>
-      <c r="F71" s="104"/>
+      <c r="E71" s="102"/>
+      <c r="F71" s="102"/>
     </row>
     <row r="72" spans="1:6" ht="88.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
@@ -21034,10 +21034,10 @@
       <c r="D114" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="107" t="s">
+      <c r="E114" s="109" t="s">
         <v>307</v>
       </c>
-      <c r="F114" s="107" t="s">
+      <c r="F114" s="109" t="s">
         <v>308</v>
       </c>
     </row>
@@ -21054,8 +21054,8 @@
       <c r="D115" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="107"/>
-      <c r="F115" s="107"/>
+      <c r="E115" s="109"/>
+      <c r="F115" s="109"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="24" t="s">
@@ -21260,10 +21260,10 @@
       <c r="D126" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E126" s="107" t="s">
+      <c r="E126" s="109" t="s">
         <v>335</v>
       </c>
-      <c r="F126" s="107" t="s">
+      <c r="F126" s="109" t="s">
         <v>336</v>
       </c>
     </row>
@@ -21280,8 +21280,8 @@
       <c r="D127" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E127" s="107"/>
-      <c r="F127" s="107"/>
+      <c r="E127" s="109"/>
+      <c r="F127" s="109"/>
     </row>
     <row r="128" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="24" t="s">
@@ -21366,10 +21366,10 @@
       <c r="D132" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E132" s="107" t="s">
+      <c r="E132" s="109" t="s">
         <v>348</v>
       </c>
-      <c r="F132" s="107" t="s">
+      <c r="F132" s="109" t="s">
         <v>349</v>
       </c>
     </row>
@@ -21386,8 +21386,8 @@
       <c r="D133" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E133" s="107"/>
-      <c r="F133" s="107"/>
+      <c r="E133" s="109"/>
+      <c r="F133" s="109"/>
     </row>
     <row r="134" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A134" s="24" t="s">
@@ -21752,10 +21752,10 @@
       <c r="D152" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E152" s="108" t="s">
+      <c r="E152" s="110" t="s">
         <v>400</v>
       </c>
-      <c r="F152" s="108" t="s">
+      <c r="F152" s="110" t="s">
         <v>401</v>
       </c>
     </row>
@@ -21772,8 +21772,8 @@
       <c r="D153" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E153" s="108"/>
-      <c r="F153" s="108"/>
+      <c r="E153" s="110"/>
+      <c r="F153" s="110"/>
     </row>
     <row r="154" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="24" t="s">
@@ -21818,10 +21818,10 @@
       <c r="D156" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E156" s="109" t="s">
+      <c r="E156" s="107" t="s">
         <v>410</v>
       </c>
-      <c r="F156" s="109" t="s">
+      <c r="F156" s="107" t="s">
         <v>411</v>
       </c>
     </row>
@@ -21838,8 +21838,8 @@
       <c r="D157" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E157" s="110"/>
-      <c r="F157" s="110"/>
+      <c r="E157" s="108"/>
+      <c r="F157" s="108"/>
     </row>
     <row r="158" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A158" s="24" t="s">
@@ -22043,6 +22043,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="F114:F115"/>
+    <mergeCell ref="F132:F133"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="F152:F153"/>
     <mergeCell ref="A155:F155"/>
     <mergeCell ref="F156:F157"/>
     <mergeCell ref="E156:E157"/>
@@ -22059,22 +22075,6 @@
     <mergeCell ref="E126:E127"/>
     <mergeCell ref="A125:F125"/>
     <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="F132:F133"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="F152:F153"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A69:F69"/>
-    <mergeCell ref="A82:F82"/>
   </mergeCells>
   <conditionalFormatting sqref="E109">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -22147,10 +22147,10 @@
       <c r="D3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="107" t="s">
+      <c r="E3" s="109" t="s">
         <v>483</v>
       </c>
-      <c r="F3" s="107" t="s">
+      <c r="F3" s="109" t="s">
         <v>484</v>
       </c>
     </row>
@@ -22167,8 +22167,8 @@
       <c r="D4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="107"/>
-      <c r="F4" s="107"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="109"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
@@ -22293,10 +22293,10 @@
       <c r="D11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="107" t="s">
+      <c r="E11" s="109" t="s">
         <v>488</v>
       </c>
-      <c r="F11" s="107" t="s">
+      <c r="F11" s="109" t="s">
         <v>489</v>
       </c>
     </row>
@@ -22313,8 +22313,8 @@
       <c r="D12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="107"/>
-      <c r="F12" s="107"/>
+      <c r="E12" s="109"/>
+      <c r="F12" s="109"/>
     </row>
     <row r="13" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -22329,8 +22329,8 @@
       <c r="D13" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="107"/>
-      <c r="F13" s="107"/>
+      <c r="E13" s="109"/>
+      <c r="F13" s="109"/>
     </row>
     <row r="14" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
@@ -23294,10 +23294,10 @@
       <c r="D64" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E64" s="107" t="s">
+      <c r="E64" s="109" t="s">
         <v>505</v>
       </c>
-      <c r="F64" s="107" t="s">
+      <c r="F64" s="109" t="s">
         <v>506</v>
       </c>
     </row>
@@ -23314,8 +23314,8 @@
       <c r="D65" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E65" s="107"/>
-      <c r="F65" s="107"/>
+      <c r="E65" s="109"/>
+      <c r="F65" s="109"/>
     </row>
     <row r="66" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="24" t="s">
@@ -23400,10 +23400,10 @@
       <c r="D70" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E70" s="107" t="s">
+      <c r="E70" s="109" t="s">
         <v>507</v>
       </c>
-      <c r="F70" s="107" t="s">
+      <c r="F70" s="109" t="s">
         <v>508</v>
       </c>
       <c r="G70" s="63"/>
@@ -23421,8 +23421,8 @@
       <c r="D71" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E71" s="107"/>
-      <c r="F71" s="107"/>
+      <c r="E71" s="109"/>
+      <c r="F71" s="109"/>
       <c r="G71" s="63"/>
     </row>
     <row r="72" spans="1:7" ht="78" x14ac:dyDescent="0.3">
@@ -24240,10 +24240,10 @@
       <c r="D114" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="111" t="s">
+      <c r="E114" s="112" t="s">
         <v>514</v>
       </c>
-      <c r="F114" s="104" t="s">
+      <c r="F114" s="102" t="s">
         <v>515</v>
       </c>
     </row>
@@ -24260,8 +24260,8 @@
       <c r="D115" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="111"/>
-      <c r="F115" s="104"/>
+      <c r="E115" s="112"/>
+      <c r="F115" s="102"/>
     </row>
     <row r="116" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="24" t="s">
@@ -24466,10 +24466,10 @@
       <c r="D126" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E126" s="104" t="s">
+      <c r="E126" s="102" t="s">
         <v>518</v>
       </c>
-      <c r="F126" s="105" t="s">
+      <c r="F126" s="103" t="s">
         <v>519</v>
       </c>
     </row>
@@ -24486,8 +24486,8 @@
       <c r="D127" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E127" s="104"/>
-      <c r="F127" s="106"/>
+      <c r="E127" s="102"/>
+      <c r="F127" s="104"/>
     </row>
     <row r="128" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A128" s="24" t="s">
@@ -24571,10 +24571,10 @@
       <c r="D132" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E132" s="104" t="s">
+      <c r="E132" s="102" t="s">
         <v>520</v>
       </c>
-      <c r="F132" s="104" t="s">
+      <c r="F132" s="102" t="s">
         <v>521</v>
       </c>
     </row>
@@ -24591,8 +24591,8 @@
       <c r="D133" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E133" s="104"/>
-      <c r="F133" s="104"/>
+      <c r="E133" s="102"/>
+      <c r="F133" s="102"/>
     </row>
     <row r="134" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A134" s="24" t="s">
@@ -24607,8 +24607,8 @@
       <c r="D134" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E134" s="104"/>
-      <c r="F134" s="104"/>
+      <c r="E134" s="102"/>
+      <c r="F134" s="102"/>
     </row>
     <row r="135" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A135" s="24" t="s">
@@ -24776,7 +24776,7 @@
       <c r="E143" s="29" t="s">
         <v>522</v>
       </c>
-      <c r="F143" s="107" t="s">
+      <c r="F143" s="109" t="s">
         <v>379</v>
       </c>
     </row>
@@ -24796,7 +24796,7 @@
       <c r="E144" s="29" t="s">
         <v>523</v>
       </c>
-      <c r="F144" s="107"/>
+      <c r="F144" s="109"/>
     </row>
     <row r="145" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A145" s="24" t="s">
@@ -24911,10 +24911,10 @@
       <c r="D150" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E150" s="105" t="s">
+      <c r="E150" s="103" t="s">
         <v>529</v>
       </c>
-      <c r="F150" s="105" t="s">
+      <c r="F150" s="103" t="s">
         <v>530</v>
       </c>
       <c r="G150" s="68"/>
@@ -24932,8 +24932,8 @@
       <c r="D151" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E151" s="106"/>
-      <c r="F151" s="106"/>
+      <c r="E151" s="104"/>
+      <c r="F151" s="104"/>
       <c r="G151" s="63"/>
     </row>
     <row r="152" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
@@ -24949,10 +24949,10 @@
       <c r="D152" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E152" s="112" t="s">
+      <c r="E152" s="111" t="s">
         <v>531</v>
       </c>
-      <c r="F152" s="112" t="s">
+      <c r="F152" s="111" t="s">
         <v>503</v>
       </c>
     </row>
@@ -24969,8 +24969,8 @@
       <c r="D153" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E153" s="112"/>
-      <c r="F153" s="112"/>
+      <c r="E153" s="111"/>
+      <c r="F153" s="111"/>
     </row>
     <row r="154" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A154" s="24" t="s">
@@ -25244,22 +25244,12 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="E152:E153"/>
-    <mergeCell ref="F152:F153"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="E132:E134"/>
-    <mergeCell ref="F132:F134"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="F143:F144"/>
-    <mergeCell ref="E150:E151"/>
-    <mergeCell ref="F150:F151"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="E114:E115"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
     <mergeCell ref="A102:F102"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="A33:F33"/>
@@ -25273,12 +25263,22 @@
     <mergeCell ref="F70:F71"/>
     <mergeCell ref="A82:F82"/>
     <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="E114:E115"/>
+    <mergeCell ref="F114:F115"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="E152:E153"/>
+    <mergeCell ref="F152:F153"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="E132:E134"/>
+    <mergeCell ref="F132:F134"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="F143:F144"/>
+    <mergeCell ref="E150:E151"/>
+    <mergeCell ref="F150:F151"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -25342,10 +25342,10 @@
       <c r="D3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="107" t="s">
+      <c r="E3" s="109" t="s">
         <v>533</v>
       </c>
-      <c r="F3" s="109" t="s">
+      <c r="F3" s="107" t="s">
         <v>534</v>
       </c>
     </row>
@@ -25362,8 +25362,8 @@
       <c r="D4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="107"/>
-      <c r="F4" s="110"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="108"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
@@ -25488,10 +25488,10 @@
       <c r="D11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="109" t="s">
+      <c r="E11" s="107" t="s">
         <v>538</v>
       </c>
-      <c r="F11" s="109" t="s">
+      <c r="F11" s="107" t="s">
         <v>539</v>
       </c>
     </row>
@@ -25508,8 +25508,8 @@
       <c r="D12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="117"/>
-      <c r="F12" s="117"/>
+      <c r="E12" s="113"/>
+      <c r="F12" s="113"/>
     </row>
     <row r="13" spans="1:6" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -25524,8 +25524,8 @@
       <c r="D13" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="110"/>
-      <c r="F13" s="110"/>
+      <c r="E13" s="108"/>
+      <c r="F13" s="108"/>
     </row>
     <row r="14" spans="1:6" ht="113.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
@@ -26590,10 +26590,10 @@
       <c r="D70" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="109" t="s">
+      <c r="E70" s="107" t="s">
         <v>549</v>
       </c>
-      <c r="F70" s="105" t="s">
+      <c r="F70" s="103" t="s">
         <v>550</v>
       </c>
     </row>
@@ -26610,8 +26610,8 @@
       <c r="D71" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E71" s="110"/>
-      <c r="F71" s="116"/>
+      <c r="E71" s="108"/>
+      <c r="F71" s="114"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
@@ -27652,10 +27652,10 @@
       <c r="D126" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E126" s="104" t="s">
+      <c r="E126" s="102" t="s">
         <v>559</v>
       </c>
-      <c r="F126" s="105" t="s">
+      <c r="F126" s="103" t="s">
         <v>560</v>
       </c>
     </row>
@@ -27672,8 +27672,8 @@
       <c r="D127" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E127" s="104"/>
-      <c r="F127" s="106"/>
+      <c r="E127" s="102"/>
+      <c r="F127" s="104"/>
     </row>
     <row r="128" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A128" s="24" t="s">
@@ -27756,10 +27756,10 @@
       <c r="D132" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E132" s="104" t="s">
+      <c r="E132" s="102" t="s">
         <v>561</v>
       </c>
-      <c r="F132" s="105" t="s">
+      <c r="F132" s="103" t="s">
         <v>562</v>
       </c>
     </row>
@@ -27776,8 +27776,8 @@
       <c r="D133" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E133" s="104"/>
-      <c r="F133" s="106"/>
+      <c r="E133" s="102"/>
+      <c r="F133" s="104"/>
     </row>
     <row r="134" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A134" s="24" t="s">
@@ -28272,10 +28272,10 @@
       <c r="D159" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E159" s="113" t="s">
+      <c r="E159" s="115" t="s">
         <v>572</v>
       </c>
-      <c r="F159" s="114" t="s">
+      <c r="F159" s="116" t="s">
         <v>573</v>
       </c>
     </row>
@@ -28292,8 +28292,8 @@
       <c r="D160" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E160" s="113"/>
-      <c r="F160" s="115"/>
+      <c r="E160" s="115"/>
+      <c r="F160" s="117"/>
     </row>
     <row r="161" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A161" s="24" t="s">
@@ -28437,12 +28437,16 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="E159:E160"/>
+    <mergeCell ref="F159:F160"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="E132:E133"/>
+    <mergeCell ref="F132:F133"/>
     <mergeCell ref="A113:F113"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="A33:F33"/>
@@ -28455,16 +28459,12 @@
     <mergeCell ref="A82:F82"/>
     <mergeCell ref="A91:F91"/>
     <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="E159:E160"/>
-    <mergeCell ref="F159:F160"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="E132:E133"/>
-    <mergeCell ref="F132:F133"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -28677,10 +28677,10 @@
       <c r="D11" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="107" t="s">
+      <c r="E11" s="109" t="s">
         <v>898</v>
       </c>
-      <c r="F11" s="107" t="s">
+      <c r="F11" s="109" t="s">
         <v>899</v>
       </c>
     </row>
@@ -28697,8 +28697,8 @@
       <c r="D12" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="107"/>
-      <c r="F12" s="107"/>
+      <c r="E12" s="109"/>
+      <c r="F12" s="109"/>
     </row>
     <row r="13" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -28843,10 +28843,10 @@
       <c r="D20" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="104" t="s">
+      <c r="E20" s="102" t="s">
         <v>904</v>
       </c>
-      <c r="F20" s="104" t="s">
+      <c r="F20" s="102" t="s">
         <v>905</v>
       </c>
     </row>
@@ -28863,8 +28863,8 @@
       <c r="D21" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="104"/>
-      <c r="F21" s="104"/>
+      <c r="E21" s="102"/>
+      <c r="F21" s="102"/>
     </row>
     <row r="22" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
@@ -29527,10 +29527,10 @@
       <c r="D56" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E56" s="107" t="s">
+      <c r="E56" s="109" t="s">
         <v>916</v>
       </c>
-      <c r="F56" s="107" t="s">
+      <c r="F56" s="109" t="s">
         <v>917</v>
       </c>
     </row>
@@ -29547,8 +29547,8 @@
       <c r="D57" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E57" s="107"/>
-      <c r="F57" s="107"/>
+      <c r="E57" s="109"/>
+      <c r="F57" s="109"/>
     </row>
     <row r="58" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A58" s="24" t="s">
@@ -29783,10 +29783,10 @@
       <c r="D70" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E70" s="107" t="s">
+      <c r="E70" s="109" t="s">
         <v>920</v>
       </c>
-      <c r="F70" s="107" t="s">
+      <c r="F70" s="109" t="s">
         <v>921</v>
       </c>
     </row>
@@ -29803,8 +29803,8 @@
       <c r="D71" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E71" s="107"/>
-      <c r="F71" s="107"/>
+      <c r="E71" s="109"/>
+      <c r="F71" s="109"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
@@ -29859,10 +29859,10 @@
       <c r="D74" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E74" s="104" t="s">
+      <c r="E74" s="102" t="s">
         <v>922</v>
       </c>
-      <c r="F74" s="104" t="s">
+      <c r="F74" s="102" t="s">
         <v>923</v>
       </c>
     </row>
@@ -29879,8 +29879,8 @@
       <c r="D75" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E75" s="104"/>
-      <c r="F75" s="104"/>
+      <c r="E75" s="102"/>
+      <c r="F75" s="102"/>
     </row>
     <row r="76" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A76" s="24" t="s">
@@ -30215,10 +30215,10 @@
       <c r="D93" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E93" s="105" t="s">
+      <c r="E93" s="103" t="s">
         <v>928</v>
       </c>
-      <c r="F93" s="105" t="s">
+      <c r="F93" s="103" t="s">
         <v>929</v>
       </c>
     </row>
@@ -30235,8 +30235,8 @@
       <c r="D94" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E94" s="106"/>
-      <c r="F94" s="106"/>
+      <c r="E94" s="104"/>
+      <c r="F94" s="104"/>
     </row>
     <row r="95" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A95" s="24" t="s">
@@ -30611,10 +30611,10 @@
       <c r="D114" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="104" t="s">
+      <c r="E114" s="102" t="s">
         <v>938</v>
       </c>
-      <c r="F114" s="104" t="s">
+      <c r="F114" s="102" t="s">
         <v>939</v>
       </c>
     </row>
@@ -30631,8 +30631,8 @@
       <c r="D115" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="104"/>
-      <c r="F115" s="104"/>
+      <c r="E115" s="102"/>
+      <c r="F115" s="102"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="24" t="s">
@@ -31176,7 +31176,7 @@
       <c r="E144" s="89" t="s">
         <v>956</v>
       </c>
-      <c r="F144" s="107" t="s">
+      <c r="F144" s="109" t="s">
         <v>40</v>
       </c>
     </row>
@@ -31196,7 +31196,7 @@
       <c r="E145" s="89" t="s">
         <v>957</v>
       </c>
-      <c r="F145" s="107"/>
+      <c r="F145" s="109"/>
     </row>
     <row r="146" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A146" s="24" t="s">
@@ -31620,15 +31620,19 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="E152:E153"/>
-    <mergeCell ref="F152:F153"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="F144:F145"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="F56:F57"/>
     <mergeCell ref="E114:E115"/>
     <mergeCell ref="F114:F115"/>
     <mergeCell ref="A69:F69"/>
@@ -31642,19 +31646,15 @@
     <mergeCell ref="F93:F94"/>
     <mergeCell ref="A102:F102"/>
     <mergeCell ref="A113:F113"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="F56:F57"/>
+    <mergeCell ref="E152:E153"/>
+    <mergeCell ref="F152:F153"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="F144:F145"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -31868,10 +31868,10 @@
       <c r="D11" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="109" t="s">
+      <c r="E11" s="107" t="s">
         <v>839</v>
       </c>
-      <c r="F11" s="107" t="s">
+      <c r="F11" s="109" t="s">
         <v>840</v>
       </c>
     </row>
@@ -31888,8 +31888,8 @@
       <c r="D12" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="110"/>
-      <c r="F12" s="107"/>
+      <c r="E12" s="108"/>
+      <c r="F12" s="109"/>
     </row>
     <row r="13" spans="1:6" ht="117" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -32034,10 +32034,10 @@
       <c r="D20" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="104" t="s">
+      <c r="E20" s="102" t="s">
         <v>845</v>
       </c>
-      <c r="F20" s="104" t="s">
+      <c r="F20" s="102" t="s">
         <v>846</v>
       </c>
     </row>
@@ -32054,8 +32054,8 @@
       <c r="D21" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="104"/>
-      <c r="F21" s="104"/>
+      <c r="E21" s="102"/>
+      <c r="F21" s="102"/>
     </row>
     <row r="22" spans="1:6" ht="118.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
@@ -32978,10 +32978,10 @@
       <c r="D70" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="109" t="s">
+      <c r="E70" s="107" t="s">
         <v>854</v>
       </c>
-      <c r="F70" s="109" t="s">
+      <c r="F70" s="107" t="s">
         <v>855</v>
       </c>
     </row>
@@ -32998,8 +32998,8 @@
       <c r="D71" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E71" s="110"/>
-      <c r="F71" s="110"/>
+      <c r="E71" s="108"/>
+      <c r="F71" s="108"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
@@ -33054,10 +33054,10 @@
       <c r="D74" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E74" s="105" t="s">
+      <c r="E74" s="103" t="s">
         <v>858</v>
       </c>
-      <c r="F74" s="105" t="s">
+      <c r="F74" s="103" t="s">
         <v>857</v>
       </c>
     </row>
@@ -33074,8 +33074,8 @@
       <c r="D75" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E75" s="106"/>
-      <c r="F75" s="106"/>
+      <c r="E75" s="104"/>
+      <c r="F75" s="104"/>
     </row>
     <row r="76" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A76" s="24" t="s">
@@ -33810,10 +33810,10 @@
       <c r="D114" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="104" t="s">
+      <c r="E114" s="102" t="s">
         <v>867</v>
       </c>
-      <c r="F114" s="105" t="s">
+      <c r="F114" s="103" t="s">
         <v>868</v>
       </c>
     </row>
@@ -33830,8 +33830,8 @@
       <c r="D115" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="104"/>
-      <c r="F115" s="106"/>
+      <c r="E115" s="102"/>
+      <c r="F115" s="104"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="24" t="s">
@@ -34825,11 +34825,24 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="E152:E153"/>
+    <mergeCell ref="E114:E115"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="F152:F153"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="F70:F71"/>
     <mergeCell ref="E20:E21"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A10:F10"/>
@@ -34837,24 +34850,11 @@
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="F20:F21"/>
     <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A69:F69"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="E152:E153"/>
-    <mergeCell ref="E114:E115"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="F152:F153"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="F114:F115"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -34918,10 +34918,10 @@
       <c r="D3" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="107" t="s">
+      <c r="E3" s="109" t="s">
         <v>768</v>
       </c>
-      <c r="F3" s="109" t="s">
+      <c r="F3" s="107" t="s">
         <v>769</v>
       </c>
     </row>
@@ -34938,8 +34938,8 @@
       <c r="D4" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="107"/>
-      <c r="F4" s="110"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="108"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
@@ -35064,10 +35064,10 @@
       <c r="D11" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="105" t="s">
+      <c r="E11" s="103" t="s">
         <v>774</v>
       </c>
-      <c r="F11" s="109" t="s">
+      <c r="F11" s="107" t="s">
         <v>775</v>
       </c>
     </row>
@@ -35084,8 +35084,8 @@
       <c r="D12" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="116"/>
-      <c r="F12" s="117"/>
+      <c r="E12" s="114"/>
+      <c r="F12" s="113"/>
     </row>
     <row r="13" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -35100,8 +35100,8 @@
       <c r="D13" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="106"/>
-      <c r="F13" s="110"/>
+      <c r="E13" s="104"/>
+      <c r="F13" s="108"/>
     </row>
     <row r="14" spans="1:6" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
@@ -35226,10 +35226,10 @@
       <c r="D20" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="107" t="s">
+      <c r="E20" s="109" t="s">
         <v>778</v>
       </c>
-      <c r="F20" s="109" t="s">
+      <c r="F20" s="107" t="s">
         <v>779</v>
       </c>
     </row>
@@ -35246,8 +35246,8 @@
       <c r="D21" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="107"/>
-      <c r="F21" s="110"/>
+      <c r="E21" s="109"/>
+      <c r="F21" s="108"/>
     </row>
     <row r="22" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
@@ -36062,10 +36062,10 @@
       <c r="D64" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E64" s="109" t="s">
+      <c r="E64" s="107" t="s">
         <v>790</v>
       </c>
-      <c r="F64" s="109" t="s">
+      <c r="F64" s="107" t="s">
         <v>791</v>
       </c>
     </row>
@@ -36082,8 +36082,8 @@
       <c r="D65" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E65" s="110"/>
-      <c r="F65" s="110"/>
+      <c r="E65" s="108"/>
+      <c r="F65" s="108"/>
     </row>
     <row r="66" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="24" t="s">
@@ -36168,10 +36168,10 @@
       <c r="D70" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E70" s="107" t="s">
+      <c r="E70" s="109" t="s">
         <v>792</v>
       </c>
-      <c r="F70" s="109" t="s">
+      <c r="F70" s="107" t="s">
         <v>793</v>
       </c>
     </row>
@@ -36188,8 +36188,8 @@
       <c r="D71" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E71" s="107"/>
-      <c r="F71" s="110"/>
+      <c r="E71" s="109"/>
+      <c r="F71" s="108"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
@@ -36244,10 +36244,10 @@
       <c r="D74" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E74" s="109" t="s">
+      <c r="E74" s="107" t="s">
         <v>794</v>
       </c>
-      <c r="F74" s="117" t="s">
+      <c r="F74" s="113" t="s">
         <v>211</v>
       </c>
     </row>
@@ -36264,8 +36264,8 @@
       <c r="D75" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E75" s="110"/>
-      <c r="F75" s="110"/>
+      <c r="E75" s="108"/>
+      <c r="F75" s="108"/>
     </row>
     <row r="76" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A76" s="24" t="s">
@@ -37000,10 +37000,10 @@
       <c r="D114" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="109" t="s">
+      <c r="E114" s="107" t="s">
         <v>805</v>
       </c>
-      <c r="F114" s="109" t="s">
+      <c r="F114" s="107" t="s">
         <v>806</v>
       </c>
     </row>
@@ -37020,8 +37020,8 @@
       <c r="D115" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="110"/>
-      <c r="F115" s="110"/>
+      <c r="E115" s="108"/>
+      <c r="F115" s="108"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="24" t="s">
@@ -38017,6 +38017,26 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="E114:E115"/>
+    <mergeCell ref="F114:F115"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="E64:E65"/>
+    <mergeCell ref="F64:F65"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="A102:F102"/>
     <mergeCell ref="A54:F54"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="E3:E4"/>
@@ -38029,26 +38049,6 @@
     <mergeCell ref="F20:F21"/>
     <mergeCell ref="A33:F33"/>
     <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="E64:E65"/>
-    <mergeCell ref="F64:F65"/>
-    <mergeCell ref="A69:F69"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="E114:E115"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -38059,8 +38059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22F8BE9-95B1-4DC7-A8A5-51C5E5B2BE2F}">
   <dimension ref="A1:F167"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E164" sqref="E164"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -38112,10 +38112,10 @@
       <c r="D3" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="109" t="s">
+      <c r="E3" s="107" t="s">
         <v>576</v>
       </c>
-      <c r="F3" s="109" t="s">
+      <c r="F3" s="107" t="s">
         <v>577</v>
       </c>
     </row>
@@ -38132,8 +38132,8 @@
       <c r="D4" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="110"/>
-      <c r="F4" s="110"/>
+      <c r="E4" s="108"/>
+      <c r="F4" s="108"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
@@ -38258,10 +38258,10 @@
       <c r="D11" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="109" t="s">
+      <c r="E11" s="107" t="s">
         <v>585</v>
       </c>
-      <c r="F11" s="109" t="s">
+      <c r="F11" s="107" t="s">
         <v>586</v>
       </c>
     </row>
@@ -38278,8 +38278,8 @@
       <c r="D12" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="117"/>
-      <c r="F12" s="117"/>
+      <c r="E12" s="113"/>
+      <c r="F12" s="113"/>
     </row>
     <row r="13" spans="1:6" ht="105.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -38294,8 +38294,8 @@
       <c r="D13" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="117"/>
-      <c r="F13" s="117"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="113"/>
     </row>
     <row r="14" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
@@ -38310,8 +38310,8 @@
       <c r="D14" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="110"/>
-      <c r="F14" s="110"/>
+      <c r="E14" s="108"/>
+      <c r="F14" s="108"/>
     </row>
     <row r="15" spans="1:6" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A15" s="24" t="s">
@@ -38416,10 +38416,10 @@
       <c r="D20" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="109" t="s">
+      <c r="E20" s="107" t="s">
         <v>587</v>
       </c>
-      <c r="F20" s="109" t="s">
+      <c r="F20" s="107" t="s">
         <v>588</v>
       </c>
     </row>
@@ -38436,8 +38436,8 @@
       <c r="D21" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="110"/>
-      <c r="F21" s="110"/>
+      <c r="E21" s="108"/>
+      <c r="F21" s="108"/>
     </row>
     <row r="22" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
@@ -39360,10 +39360,10 @@
       <c r="D70" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E70" s="109" t="s">
+      <c r="E70" s="107" t="s">
         <v>596</v>
       </c>
-      <c r="F70" s="109" t="s">
+      <c r="F70" s="107" t="s">
         <v>597</v>
       </c>
     </row>
@@ -39380,8 +39380,8 @@
       <c r="D71" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E71" s="110"/>
-      <c r="F71" s="110"/>
+      <c r="E71" s="108"/>
+      <c r="F71" s="108"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
@@ -39436,10 +39436,10 @@
       <c r="D74" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E74" s="104" t="s">
+      <c r="E74" s="102" t="s">
         <v>599</v>
       </c>
-      <c r="F74" s="104" t="s">
+      <c r="F74" s="102" t="s">
         <v>599</v>
       </c>
     </row>
@@ -39456,8 +39456,8 @@
       <c r="D75" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E75" s="104"/>
-      <c r="F75" s="104"/>
+      <c r="E75" s="102"/>
+      <c r="F75" s="102"/>
     </row>
     <row r="76" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A76" s="24" t="s">
@@ -39790,10 +39790,10 @@
       <c r="D93" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E93" s="109" t="s">
+      <c r="E93" s="107" t="s">
         <v>607</v>
       </c>
-      <c r="F93" s="109" t="s">
+      <c r="F93" s="107" t="s">
         <v>594</v>
       </c>
     </row>
@@ -39810,8 +39810,8 @@
       <c r="D94" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E94" s="110"/>
-      <c r="F94" s="110"/>
+      <c r="E94" s="108"/>
+      <c r="F94" s="108"/>
     </row>
     <row r="95" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A95" s="24" t="s">
@@ -40186,10 +40186,10 @@
       <c r="D114" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="107" t="s">
+      <c r="E114" s="109" t="s">
         <v>614</v>
       </c>
-      <c r="F114" s="109" t="s">
+      <c r="F114" s="107" t="s">
         <v>615</v>
       </c>
     </row>
@@ -40206,8 +40206,8 @@
       <c r="D115" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="107"/>
-      <c r="F115" s="110"/>
+      <c r="E115" s="109"/>
+      <c r="F115" s="108"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="24" t="s">
@@ -41203,6 +41203,26 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="E114:E115"/>
+    <mergeCell ref="F114:F115"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="E93:E94"/>
+    <mergeCell ref="F93:F94"/>
+    <mergeCell ref="A102:F102"/>
     <mergeCell ref="A54:F54"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="E3:E4"/>
@@ -41215,26 +41235,6 @@
     <mergeCell ref="F20:F21"/>
     <mergeCell ref="A33:F33"/>
     <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A69:F69"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="E93:E94"/>
-    <mergeCell ref="F93:F94"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="E114:E115"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>